<commit_message>
criação das escalas novas
</commit_message>
<xml_diff>
--- a/planilha/Escala ASO1 - Cidade Industrial - 1° Turno - Novembro.xlsx
+++ b/planilha/Escala ASO1 - Cidade Industrial - 1° Turno - Novembro.xlsx
@@ -31,13 +31,13 @@
     <t>S</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Q</t>
   </si>
   <si>
     <t>B1</t>
@@ -553,110 +553,106 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC2" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD2" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AE2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="AG2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="AH2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="AI2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="U2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="V2" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="W2" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="X2" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="Y2" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AA2" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AB2" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AC2" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AE2" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="AF2" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="AG2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AK2" s="1" t="n">
-        <v>5</v>
-      </c>
+      <c r="AJ2" s="1" t="n"/>
+      <c r="AK2" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="3" spans="1:48">
       <c r="A3" s="1" t="s"/>
@@ -670,19 +666,19 @@
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>3</v>
@@ -691,19 +687,19 @@
         <v>4</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>3</v>
@@ -712,19 +708,19 @@
         <v>4</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>3</v>
@@ -733,19 +729,19 @@
         <v>4</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="AE3" s="1" t="s">
         <v>3</v>
@@ -754,20 +750,16 @@
         <v>4</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AK3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="AJ3" s="1" t="n"/>
+      <c r="AK3" s="1" t="n"/>
       <c r="AM3" t="s">
         <v>7</v>
       </c>
@@ -809,8 +801,8 @@
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
@@ -818,99 +810,95 @@
       <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>19</v>
+      <c r="G4" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>8</v>
+      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>7</v>
+      <c r="M4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>7</v>
+      <c r="T4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="3" t="s">
-        <v>7</v>
+      <c r="Y4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="AC4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AD4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>13</v>
+      <c r="AD4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ4" s="3" t="n"/>
+      <c r="AK4" s="3" t="n"/>
       <c r="AM4">
         <f>COUNTIF(B4:AG4; "B1")</f>
         <v/>
@@ -959,111 +947,107 @@
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>19</v>
+      <c r="J5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>8</v>
+      <c r="M5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>8</v>
+        <v>8</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="Y5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Z5" s="4" t="s">
-        <v>19</v>
+      <c r="Z5" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC5" s="5" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AD5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AE5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>19</v>
+      <c r="AE5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="AG5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AH5" s="5" t="s">
-        <v>8</v>
+      <c r="AH5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AI5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK5" s="5" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="AJ5" s="5" t="n"/>
+      <c r="AK5" s="5" t="n"/>
       <c r="AM5">
         <f>COUNTIF(B5:AG5; "B1")</f>
         <v/>
@@ -1112,111 +1096,107 @@
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>13</v>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>19</v>
+      <c r="J6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>7</v>
+      <c r="M6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="U6" s="4" t="s">
-        <v>19</v>
+      <c r="U6" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="V6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>7</v>
+      <c r="W6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>13</v>
+      <c r="AA6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF6" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="AG6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AH6" s="3" t="s">
-        <v>13</v>
+      <c r="AH6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AI6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AJ6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK6" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="AJ6" s="3" t="n"/>
+      <c r="AK6" s="3" t="n"/>
       <c r="AM6">
         <f>COUNTIF(B6:AG6; "B1")</f>
         <v/>
@@ -1265,85 +1245,87 @@
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5" t="s"/>
-      <c r="D7" s="5" t="s"/>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="E7" s="5" t="s"/>
-      <c r="F7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>7</v>
+      <c r="F7" s="5" t="s"/>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="5" t="s"/>
-      <c r="J7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="I7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="5" t="s"/>
       <c r="L7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" s="5" t="s"/>
+      <c r="M7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="O7" s="5" t="s"/>
-      <c r="P7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>8</v>
+      <c r="P7" s="5" t="s"/>
+      <c r="Q7" s="5" t="s"/>
+      <c r="R7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="S7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="T7" s="5" t="s"/>
-      <c r="U7" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="T7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="5" t="s"/>
       <c r="V7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="5" t="s"/>
-      <c r="Y7" s="5" t="s"/>
+      <c r="W7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="Z7" s="5" t="s"/>
-      <c r="AA7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB7" s="5" t="s">
-        <v>7</v>
+      <c r="AA7" s="5" t="s"/>
+      <c r="AB7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD7" s="5" t="s"/>
-      <c r="AE7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF7" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF7" s="5" t="s"/>
       <c r="AG7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AH7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI7" s="5" t="s"/>
-      <c r="AJ7" s="5" t="s"/>
-      <c r="AK7" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="AH7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ7" s="5" t="n"/>
+      <c r="AK7" s="5" t="n"/>
       <c r="AM7">
         <f>COUNTIF(B7:AG7; "B1")</f>
         <v/>
@@ -1392,89 +1374,85 @@
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3" t="s"/>
-      <c r="G8" s="3" t="s"/>
-      <c r="H8" s="4" t="s">
-        <v>19</v>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s"/>
+      <c r="E8" s="3" t="s"/>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="3" t="s"/>
-      <c r="M8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="J8" s="3" t="s"/>
+      <c r="K8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="3" t="s"/>
+      <c r="O8" s="3" t="s"/>
       <c r="P8" s="3" t="s"/>
-      <c r="Q8" s="3" t="s"/>
-      <c r="R8" s="3" t="s"/>
-      <c r="S8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="V8" s="3" t="s"/>
+      <c r="Q8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" s="3" t="s"/>
+      <c r="U8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="W8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA8" s="3" t="s"/>
-      <c r="AB8" s="3" t="s"/>
-      <c r="AC8" s="4" t="s">
-        <v>19</v>
+      <c r="X8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y8" s="3" t="s"/>
+      <c r="Z8" s="3" t="s"/>
+      <c r="AA8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="AD8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AE8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG8" s="3" t="s"/>
-      <c r="AH8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AK8" s="3" t="s"/>
+      <c r="AE8" s="3" t="s"/>
+      <c r="AF8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI8" s="3" t="s"/>
+      <c r="AJ8" s="3" t="n"/>
+      <c r="AK8" s="3" t="n"/>
       <c r="AM8">
         <f>COUNTIF(B8:AG8; "B1")</f>
         <v/>
@@ -1523,65 +1501,63 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s"/>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D9" s="5" t="s"/>
       <c r="E9" s="5" t="s"/>
-      <c r="F9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="5" t="s"/>
+      <c r="F9" s="5" t="s"/>
+      <c r="G9" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="H9" s="5" t="s"/>
       <c r="I9" s="5" t="s"/>
-      <c r="J9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="J9" s="5" t="s"/>
+      <c r="K9" s="5" t="s"/>
       <c r="L9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="5" t="s"/>
+      <c r="M9" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="N9" s="5" t="s"/>
       <c r="O9" s="5" t="s"/>
-      <c r="P9" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="P9" s="5" t="s"/>
       <c r="Q9" s="5" t="s"/>
-      <c r="R9" s="5" t="s"/>
+      <c r="R9" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="S9" s="5" t="s"/>
       <c r="T9" s="5" t="s"/>
-      <c r="U9" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="U9" s="5" t="s"/>
       <c r="V9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="W9" s="5" t="s"/>
-      <c r="X9" s="5" t="s"/>
+        <v>7</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="Y9" s="5" t="s"/>
       <c r="Z9" s="5" t="s"/>
-      <c r="AA9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB9" s="5" t="s"/>
+      <c r="AA9" s="5" t="s"/>
+      <c r="AB9" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="AC9" s="5" t="s"/>
       <c r="AD9" s="5" t="s"/>
-      <c r="AE9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF9" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="AE9" s="5" t="s"/>
+      <c r="AF9" s="5" t="s"/>
       <c r="AG9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH9" s="5" t="s"/>
+        <v>13</v>
+      </c>
+      <c r="AH9" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="AI9" s="5" t="s"/>
-      <c r="AJ9" s="5" t="s"/>
-      <c r="AK9" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="AJ9" s="5" t="n"/>
+      <c r="AK9" s="5" t="n"/>
       <c r="AM9">
         <f>COUNTIF(B9:AG9; "B1")</f>
         <v/>

</xml_diff>